<commit_message>
Separated build from tools
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-saner-bed-group.xlsx
+++ b/docs/StructureDefinition-saner-bed-group.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AK$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AK$87</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3028" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2892" uniqueCount="334">
   <si>
     <t>Path</t>
   </si>
@@ -918,33 +918,35 @@
     <t>Status</t>
   </si>
   <si>
+    <t>The Status slice reports on the status of the bed (e.g., active | suspended | inactive)</t>
+  </si>
+  <si>
+    <t>An active bed is one that can be used, suspended is one that has been temporarily taken out of service, an inactive one is not available</t>
+  </si>
+  <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
   &lt;coding&gt;
-    &lt;system value="http://hl7.org/fhir/location-definitions.html"/&gt;
+    &lt;system value="http://hl7.org/fhir/R4/StructureDefinition/Location"/&gt;
     &lt;code value="Location.status"/&gt;
   &lt;/coding&gt;
 &lt;/valueCodeableConcept&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">type:$this}
-</t>
-  </si>
-  <si>
-    <t>closed</t>
-  </si>
-  <si>
-    <t>valueCodeableConcept</t>
-  </si>
-  <si>
     <t>http://hl7.org/fhir/ValueSet/location-status</t>
   </si>
   <si>
     <t>OperationalStatus</t>
+  </si>
+  <si>
+    <t>The OperationalStatus slice reports on the operationalStatus of the bed (e.g., occupied | unoccupied | housekeeping)</t>
+  </si>
+  <si>
+    <t>OperationalStatus helps assess whether a bed is in use or could be placed into use</t>
   </si>
   <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
   &lt;coding&gt;
-    &lt;system value="http://hl7.org/fhir/location-definitions.html"/&gt;
+    &lt;system value="http://hl7.org/fhir/R4/StructureDefinition/Location"/&gt;
     &lt;code value="Location.operationalStatus"/&gt;
   &lt;/coding&gt;
 &lt;/valueCodeableConcept&gt;</t>
@@ -956,43 +958,61 @@
     <t>Type</t>
   </si>
   <si>
+    <t>The Type slice reports on the type location for the bed (e.g., ICU | ER| Hospital Unit)</t>
+  </si>
+  <si>
+    <t>Type helps to identify the services available to patients using the bed</t>
+  </si>
+  <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
   &lt;coding&gt;
-    &lt;system value="http://hl7.org/fhir/location-definitions.html"/&gt;
+    &lt;system value="http://hl7.org/fhir/R4/StructureDefinition/Location"/&gt;
     &lt;code value="Location.type"/&gt;
   &lt;/coding&gt;
 &lt;/valueCodeableConcept&gt;</t>
   </si>
   <si>
-    <t>http://terminology.hl7.org/ValueSet/v3-ServiceDeliveryLocationRoleType</t>
-  </si>
-  <si>
-    <t>Feature</t>
+    <t>http://ainq.com/fhir/us/saner/ValueSet/BedType</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>The Property slice reports on isolation properties of the bed(e.g., NEGISO | OTHISO | NONISO)</t>
+  </si>
+  <si>
+    <t>Property identifies important properties of the bed (e.g., isolation)</t>
   </si>
   <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
   &lt;coding&gt;
-    &lt;system value="http://hl7.org/fhir/location-definitions.html"/&gt;
+    &lt;system value="http://hl7.org/fhir/R4/StructureDefinition/Location"/&gt;
     &lt;code value="Location.Feature"/&gt;
   &lt;/coding&gt;
 &lt;/valueCodeableConcept&gt;</t>
   </si>
   <si>
-    <t>http://ainq.com/fhir/us/saner/ValueSet/BedFeature</t>
+    <t>http://ainq.com/fhir/us/saner/ValueSet/BedProperty</t>
   </si>
   <si>
     <t>Location</t>
+  </si>
+  <si>
+    <t>The Location slice reports the physical location of the bed (e.g., address, GPS coordinates)</t>
+  </si>
+  <si>
+    <t>Location aids in mapping, navigation and communications to or about the bed.</t>
   </si>
   <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
   &lt;coding&gt;
-    &lt;system value="http://hl7.org/fhir/location-definitions.html"/&gt;
+    &lt;system value="http://hl7.org/fhir/R4/StructureDefinition/Location"/&gt;
     &lt;code value="Location.partOf"/&gt;
   &lt;/coding&gt;
 &lt;/valueCodeableConcept&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Location)
+    <t xml:space="preserve">Reference(http://ainq.com/fhir/us/saner/StructureDefinition/saner-resource-location)
 </t>
   </si>
   <si>
@@ -1209,7 +1229,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AK91"/>
+  <dimension ref="A1:AK87"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1219,7 +1239,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="39.19140625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="21.63671875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="17.234375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
@@ -1228,7 +1248,7 @@
     <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="58.69921875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="105.9921875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1242,7 +1262,7 @@
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="95.56640625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="66.81640625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="64.8515625" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="41.81640625" customWidth="true" bestFit="true"/>
@@ -5505,13 +5525,13 @@
         <v>249</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>250</v>
+        <v>288</v>
       </c>
       <c r="L41" t="s" s="2">
         <v>251</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>252</v>
+        <v>289</v>
       </c>
       <c r="N41" t="s" s="2">
         <v>253</v>
@@ -5944,7 +5964,7 @@
         <v>38</v>
       </c>
       <c r="R45" t="s" s="2">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="S45" t="s" s="2">
         <v>38</v>
@@ -6066,26 +6086,26 @@
         <v>38</v>
       </c>
       <c r="W46" t="s" s="2">
-        <v>143</v>
-      </c>
-      <c r="X46" t="s" s="2">
-        <v>275</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="X46" s="2"/>
       <c r="Y46" t="s" s="2">
-        <v>38</v>
+        <v>291</v>
       </c>
       <c r="Z46" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AA46" t="s" s="2">
-        <v>289</v>
-      </c>
-      <c r="AB46" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="AB46" t="s" s="2">
+        <v>38</v>
+      </c>
       <c r="AC46" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AD46" t="s" s="2">
-        <v>290</v>
+        <v>38</v>
       </c>
       <c r="AE46" t="s" s="2">
         <v>269</v>
@@ -6111,17 +6131,15 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="B47" t="s" s="2">
-        <v>291</v>
-      </c>
+        <v>277</v>
+      </c>
+      <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
         <v>38</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F47" t="s" s="2">
         <v>47</v>
@@ -6136,19 +6154,19 @@
         <v>38</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="N47" t="s" s="2">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>38</v>
@@ -6173,11 +6191,13 @@
         <v>38</v>
       </c>
       <c r="W47" t="s" s="2">
-        <v>125</v>
-      </c>
-      <c r="X47" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="X47" t="s" s="2">
+        <v>38</v>
+      </c>
       <c r="Y47" t="s" s="2">
-        <v>292</v>
+        <v>38</v>
       </c>
       <c r="Z47" t="s" s="2">
         <v>38</v>
@@ -6195,7 +6215,7 @@
         <v>38</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>47</v>
@@ -6210,7 +6230,7 @@
         <v>59</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="AK47" t="s" s="2">
         <v>38</v>
@@ -6218,7 +6238,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -6226,7 +6246,7 @@
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F48" t="s" s="2">
         <v>47</v>
@@ -6241,20 +6261,16 @@
         <v>38</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>112</v>
+        <v>231</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>279</v>
-      </c>
-      <c r="M48" t="s" s="2">
-        <v>280</v>
-      </c>
-      <c r="N48" t="s" s="2">
-        <v>281</v>
-      </c>
+        <v>286</v>
+      </c>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
         <v>38</v>
       </c>
@@ -6302,10 +6318,10 @@
         <v>38</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>47</v>
@@ -6317,7 +6333,7 @@
         <v>59</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>283</v>
+        <v>38</v>
       </c>
       <c r="AK48" t="s" s="2">
         <v>38</v>
@@ -6325,15 +6341,17 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>284</v>
-      </c>
-      <c r="B49" s="2"/>
+        <v>247</v>
+      </c>
+      <c r="B49" t="s" s="2">
+        <v>292</v>
+      </c>
       <c r="C49" t="s" s="2">
         <v>38</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F49" t="s" s="2">
         <v>47</v>
@@ -6348,16 +6366,20 @@
         <v>38</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>231</v>
+        <v>249</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>286</v>
-      </c>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
+        <v>251</v>
+      </c>
+      <c r="M49" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="N49" t="s" s="2">
+        <v>253</v>
+      </c>
       <c r="O49" t="s" s="2">
         <v>38</v>
       </c>
@@ -6405,13 +6427,13 @@
         <v>38</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>284</v>
+        <v>247</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG49" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AH49" t="s" s="2">
         <v>38</v>
@@ -6420,7 +6442,7 @@
         <v>59</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>38</v>
+        <v>256</v>
       </c>
       <c r="AK49" t="s" s="2">
         <v>38</v>
@@ -6428,17 +6450,15 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>247</v>
-      </c>
-      <c r="B50" t="s" s="2">
-        <v>293</v>
-      </c>
+        <v>257</v>
+      </c>
+      <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
         <v>38</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F50" t="s" s="2">
         <v>47</v>
@@ -6453,20 +6473,16 @@
         <v>38</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>249</v>
+        <v>49</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>250</v>
+        <v>165</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>251</v>
-      </c>
-      <c r="M50" t="s" s="2">
-        <v>252</v>
-      </c>
-      <c r="N50" t="s" s="2">
-        <v>253</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
       <c r="O50" t="s" s="2">
         <v>38</v>
       </c>
@@ -6514,22 +6530,22 @@
         <v>38</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>247</v>
+        <v>167</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG50" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="AH50" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AI50" t="s" s="2">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>256</v>
+        <v>168</v>
       </c>
       <c r="AK50" t="s" s="2">
         <v>38</v>
@@ -6537,18 +6553,18 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F51" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G51" t="s" s="2">
         <v>38</v>
@@ -6560,15 +6576,17 @@
         <v>38</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>165</v>
+        <v>94</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>166</v>
-      </c>
-      <c r="M51" s="2"/>
+        <v>170</v>
+      </c>
+      <c r="M51" t="s" s="2">
+        <v>96</v>
+      </c>
       <c r="N51" s="2"/>
       <c r="O51" t="s" s="2">
         <v>38</v>
@@ -6617,19 +6635,19 @@
         <v>38</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG51" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AH51" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AI51" t="s" s="2">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="AJ51" t="s" s="2">
         <v>168</v>
@@ -6640,11 +6658,11 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
-        <v>92</v>
+        <v>260</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" t="s" s="2">
@@ -6657,24 +6675,26 @@
         <v>38</v>
       </c>
       <c r="H52" t="s" s="2">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="I52" t="s" s="2">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="J52" t="s" s="2">
         <v>93</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>94</v>
+        <v>261</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>170</v>
+        <v>262</v>
       </c>
       <c r="M52" t="s" s="2">
         <v>96</v>
       </c>
-      <c r="N52" s="2"/>
+      <c r="N52" t="s" s="2">
+        <v>102</v>
+      </c>
       <c r="O52" t="s" s="2">
         <v>38</v>
       </c>
@@ -6722,7 +6742,7 @@
         <v>38</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>174</v>
+        <v>263</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>39</v>
@@ -6737,7 +6757,7 @@
         <v>98</v>
       </c>
       <c r="AJ52" t="s" s="2">
-        <v>168</v>
+        <v>90</v>
       </c>
       <c r="AK52" t="s" s="2">
         <v>38</v>
@@ -6745,42 +6765,40 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
-        <v>260</v>
+        <v>38</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F53" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="G53" t="s" s="2">
         <v>38</v>
       </c>
       <c r="H53" t="s" s="2">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="I53" t="s" s="2">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>93</v>
+        <v>138</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>262</v>
-      </c>
-      <c r="M53" t="s" s="2">
-        <v>96</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="M53" s="2"/>
       <c r="N53" t="s" s="2">
-        <v>102</v>
+        <v>267</v>
       </c>
       <c r="O53" t="s" s="2">
         <v>38</v>
@@ -6790,7 +6808,7 @@
         <v>38</v>
       </c>
       <c r="R53" t="s" s="2">
-        <v>38</v>
+        <v>295</v>
       </c>
       <c r="S53" t="s" s="2">
         <v>38</v>
@@ -6805,10 +6823,10 @@
         <v>38</v>
       </c>
       <c r="W53" t="s" s="2">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="X53" t="s" s="2">
-        <v>38</v>
+        <v>268</v>
       </c>
       <c r="Y53" t="s" s="2">
         <v>38</v>
@@ -6829,22 +6847,22 @@
         <v>38</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="AG53" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="AH53" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AI53" t="s" s="2">
-        <v>98</v>
+        <v>59</v>
       </c>
       <c r="AJ53" t="s" s="2">
-        <v>90</v>
+        <v>145</v>
       </c>
       <c r="AK53" t="s" s="2">
         <v>38</v>
@@ -6852,7 +6870,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -6878,14 +6896,16 @@
         <v>138</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>266</v>
-      </c>
-      <c r="M54" s="2"/>
+        <v>272</v>
+      </c>
+      <c r="M54" t="s" s="2">
+        <v>273</v>
+      </c>
       <c r="N54" t="s" s="2">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="O54" t="s" s="2">
         <v>38</v>
@@ -6895,7 +6915,7 @@
         <v>38</v>
       </c>
       <c r="R54" t="s" s="2">
-        <v>294</v>
+        <v>38</v>
       </c>
       <c r="S54" t="s" s="2">
         <v>38</v>
@@ -6910,13 +6930,11 @@
         <v>38</v>
       </c>
       <c r="W54" t="s" s="2">
-        <v>143</v>
-      </c>
-      <c r="X54" t="s" s="2">
-        <v>268</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="X54" s="2"/>
       <c r="Y54" t="s" s="2">
-        <v>38</v>
+        <v>296</v>
       </c>
       <c r="Z54" t="s" s="2">
         <v>38</v>
@@ -6934,7 +6952,7 @@
         <v>38</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>47</v>
@@ -6949,7 +6967,7 @@
         <v>59</v>
       </c>
       <c r="AJ54" t="s" s="2">
-        <v>145</v>
+        <v>276</v>
       </c>
       <c r="AK54" t="s" s="2">
         <v>38</v>
@@ -6957,7 +6975,7 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -6980,19 +6998,19 @@
         <v>38</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="N55" t="s" s="2">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="O55" t="s" s="2">
         <v>38</v>
@@ -7017,10 +7035,10 @@
         <v>38</v>
       </c>
       <c r="W55" t="s" s="2">
-        <v>143</v>
+        <v>38</v>
       </c>
       <c r="X55" t="s" s="2">
-        <v>275</v>
+        <v>38</v>
       </c>
       <c r="Y55" t="s" s="2">
         <v>38</v>
@@ -7029,17 +7047,19 @@
         <v>38</v>
       </c>
       <c r="AA55" t="s" s="2">
-        <v>289</v>
-      </c>
-      <c r="AB55" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="AB55" t="s" s="2">
+        <v>38</v>
+      </c>
       <c r="AC55" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AD55" t="s" s="2">
-        <v>290</v>
+        <v>38</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>47</v>
@@ -7054,7 +7074,7 @@
         <v>59</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="AK55" t="s" s="2">
         <v>38</v>
@@ -7062,11 +7082,9 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="B56" t="s" s="2">
-        <v>291</v>
-      </c>
+        <v>284</v>
+      </c>
+      <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
         <v>38</v>
       </c>
@@ -7087,20 +7105,16 @@
         <v>38</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>138</v>
+        <v>231</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>272</v>
-      </c>
-      <c r="M56" t="s" s="2">
-        <v>273</v>
-      </c>
-      <c r="N56" t="s" s="2">
-        <v>274</v>
-      </c>
+        <v>286</v>
+      </c>
+      <c r="M56" s="2"/>
+      <c r="N56" s="2"/>
       <c r="O56" t="s" s="2">
         <v>38</v>
       </c>
@@ -7124,11 +7138,13 @@
         <v>38</v>
       </c>
       <c r="W56" t="s" s="2">
-        <v>125</v>
-      </c>
-      <c r="X56" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="X56" t="s" s="2">
+        <v>38</v>
+      </c>
       <c r="Y56" t="s" s="2">
-        <v>295</v>
+        <v>38</v>
       </c>
       <c r="Z56" t="s" s="2">
         <v>38</v>
@@ -7146,10 +7162,10 @@
         <v>38</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>269</v>
+        <v>284</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>47</v>
@@ -7161,7 +7177,7 @@
         <v>59</v>
       </c>
       <c r="AJ56" t="s" s="2">
-        <v>276</v>
+        <v>38</v>
       </c>
       <c r="AK56" t="s" s="2">
         <v>38</v>
@@ -7169,9 +7185,11 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>277</v>
-      </c>
-      <c r="B57" s="2"/>
+        <v>247</v>
+      </c>
+      <c r="B57" t="s" s="2">
+        <v>297</v>
+      </c>
       <c r="C57" t="s" s="2">
         <v>38</v>
       </c>
@@ -7192,19 +7210,19 @@
         <v>38</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>112</v>
+        <v>249</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>279</v>
+        <v>251</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>280</v>
+        <v>299</v>
       </c>
       <c r="N57" t="s" s="2">
-        <v>281</v>
+        <v>253</v>
       </c>
       <c r="O57" t="s" s="2">
         <v>38</v>
@@ -7253,13 +7271,13 @@
         <v>38</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>277</v>
+        <v>247</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="AG57" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AH57" t="s" s="2">
         <v>38</v>
@@ -7268,7 +7286,7 @@
         <v>59</v>
       </c>
       <c r="AJ57" t="s" s="2">
-        <v>283</v>
+        <v>256</v>
       </c>
       <c r="AK57" t="s" s="2">
         <v>38</v>
@@ -7276,7 +7294,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>284</v>
+        <v>257</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -7299,13 +7317,13 @@
         <v>38</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>231</v>
+        <v>49</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>285</v>
+        <v>165</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>286</v>
+        <v>166</v>
       </c>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -7356,7 +7374,7 @@
         <v>38</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>284</v>
+        <v>167</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>39</v>
@@ -7368,10 +7386,10 @@
         <v>38</v>
       </c>
       <c r="AI58" t="s" s="2">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="AJ58" t="s" s="2">
-        <v>38</v>
+        <v>168</v>
       </c>
       <c r="AK58" t="s" s="2">
         <v>38</v>
@@ -7379,20 +7397,18 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>247</v>
-      </c>
-      <c r="B59" t="s" s="2">
-        <v>296</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F59" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G59" t="s" s="2">
         <v>38</v>
@@ -7404,20 +7420,18 @@
         <v>38</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>249</v>
+        <v>93</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>250</v>
+        <v>94</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>251</v>
+        <v>170</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>252</v>
-      </c>
-      <c r="N59" t="s" s="2">
-        <v>253</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="N59" s="2"/>
       <c r="O59" t="s" s="2">
         <v>38</v>
       </c>
@@ -7465,7 +7479,7 @@
         <v>38</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>247</v>
+        <v>174</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>39</v>
@@ -7477,10 +7491,10 @@
         <v>38</v>
       </c>
       <c r="AI59" t="s" s="2">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>256</v>
+        <v>168</v>
       </c>
       <c r="AK59" t="s" s="2">
         <v>38</v>
@@ -7488,39 +7502,43 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
-        <v>38</v>
+        <v>260</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F60" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G60" t="s" s="2">
         <v>38</v>
       </c>
       <c r="H60" t="s" s="2">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="I60" t="s" s="2">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>165</v>
+        <v>261</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>166</v>
-      </c>
-      <c r="M60" s="2"/>
-      <c r="N60" s="2"/>
+        <v>262</v>
+      </c>
+      <c r="M60" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="N60" t="s" s="2">
+        <v>102</v>
+      </c>
       <c r="O60" t="s" s="2">
         <v>38</v>
       </c>
@@ -7568,22 +7586,22 @@
         <v>38</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>167</v>
+        <v>263</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG60" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AH60" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AI60" t="s" s="2">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="AJ60" t="s" s="2">
-        <v>168</v>
+        <v>90</v>
       </c>
       <c r="AK60" t="s" s="2">
         <v>38</v>
@@ -7591,18 +7609,18 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
-        <v>92</v>
+        <v>38</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F61" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="G61" t="s" s="2">
         <v>38</v>
@@ -7614,18 +7632,18 @@
         <v>38</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>93</v>
+        <v>138</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>94</v>
+        <v>265</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>170</v>
-      </c>
-      <c r="M61" t="s" s="2">
-        <v>96</v>
-      </c>
-      <c r="N61" s="2"/>
+        <v>266</v>
+      </c>
+      <c r="M61" s="2"/>
+      <c r="N61" t="s" s="2">
+        <v>267</v>
+      </c>
       <c r="O61" t="s" s="2">
         <v>38</v>
       </c>
@@ -7634,7 +7652,7 @@
         <v>38</v>
       </c>
       <c r="R61" t="s" s="2">
-        <v>38</v>
+        <v>300</v>
       </c>
       <c r="S61" t="s" s="2">
         <v>38</v>
@@ -7649,10 +7667,10 @@
         <v>38</v>
       </c>
       <c r="W61" t="s" s="2">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="X61" t="s" s="2">
-        <v>38</v>
+        <v>268</v>
       </c>
       <c r="Y61" t="s" s="2">
         <v>38</v>
@@ -7673,22 +7691,22 @@
         <v>38</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>174</v>
+        <v>264</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="AG61" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="AH61" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AI61" t="s" s="2">
-        <v>98</v>
+        <v>59</v>
       </c>
       <c r="AJ61" t="s" s="2">
-        <v>168</v>
+        <v>145</v>
       </c>
       <c r="AK61" t="s" s="2">
         <v>38</v>
@@ -7696,42 +7714,42 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>259</v>
+        <v>269</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
-        <v>260</v>
+        <v>38</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F62" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="G62" t="s" s="2">
         <v>38</v>
       </c>
       <c r="H62" t="s" s="2">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="I62" t="s" s="2">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>93</v>
+        <v>138</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>96</v>
+        <v>273</v>
       </c>
       <c r="N62" t="s" s="2">
-        <v>102</v>
+        <v>274</v>
       </c>
       <c r="O62" t="s" s="2">
         <v>38</v>
@@ -7756,13 +7774,11 @@
         <v>38</v>
       </c>
       <c r="W62" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="X62" t="s" s="2">
-        <v>38</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="X62" s="2"/>
       <c r="Y62" t="s" s="2">
-        <v>38</v>
+        <v>301</v>
       </c>
       <c r="Z62" t="s" s="2">
         <v>38</v>
@@ -7780,22 +7796,22 @@
         <v>38</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="AF62" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="AG62" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="AH62" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AI62" t="s" s="2">
-        <v>98</v>
+        <v>59</v>
       </c>
       <c r="AJ62" t="s" s="2">
-        <v>90</v>
+        <v>276</v>
       </c>
       <c r="AK62" t="s" s="2">
         <v>38</v>
@@ -7803,7 +7819,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>264</v>
+        <v>277</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -7826,17 +7842,19 @@
         <v>38</v>
       </c>
       <c r="J63" t="s" s="2">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>265</v>
+        <v>278</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>266</v>
-      </c>
-      <c r="M63" s="2"/>
+        <v>279</v>
+      </c>
+      <c r="M63" t="s" s="2">
+        <v>280</v>
+      </c>
       <c r="N63" t="s" s="2">
-        <v>267</v>
+        <v>281</v>
       </c>
       <c r="O63" t="s" s="2">
         <v>38</v>
@@ -7846,7 +7864,7 @@
         <v>38</v>
       </c>
       <c r="R63" t="s" s="2">
-        <v>297</v>
+        <v>38</v>
       </c>
       <c r="S63" t="s" s="2">
         <v>38</v>
@@ -7861,10 +7879,10 @@
         <v>38</v>
       </c>
       <c r="W63" t="s" s="2">
-        <v>143</v>
+        <v>38</v>
       </c>
       <c r="X63" t="s" s="2">
-        <v>268</v>
+        <v>38</v>
       </c>
       <c r="Y63" t="s" s="2">
         <v>38</v>
@@ -7885,7 +7903,7 @@
         <v>38</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>264</v>
+        <v>277</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>47</v>
@@ -7900,7 +7918,7 @@
         <v>59</v>
       </c>
       <c r="AJ63" t="s" s="2">
-        <v>145</v>
+        <v>283</v>
       </c>
       <c r="AK63" t="s" s="2">
         <v>38</v>
@@ -7908,7 +7926,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>269</v>
+        <v>284</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -7916,7 +7934,7 @@
       </c>
       <c r="D64" s="2"/>
       <c r="E64" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F64" t="s" s="2">
         <v>47</v>
@@ -7931,20 +7949,16 @@
         <v>38</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>138</v>
+        <v>231</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>272</v>
-      </c>
-      <c r="M64" t="s" s="2">
-        <v>273</v>
-      </c>
-      <c r="N64" t="s" s="2">
-        <v>274</v>
-      </c>
+        <v>286</v>
+      </c>
+      <c r="M64" s="2"/>
+      <c r="N64" s="2"/>
       <c r="O64" t="s" s="2">
         <v>38</v>
       </c>
@@ -7968,10 +7982,10 @@
         <v>38</v>
       </c>
       <c r="W64" t="s" s="2">
-        <v>143</v>
+        <v>38</v>
       </c>
       <c r="X64" t="s" s="2">
-        <v>275</v>
+        <v>38</v>
       </c>
       <c r="Y64" t="s" s="2">
         <v>38</v>
@@ -7980,20 +7994,22 @@
         <v>38</v>
       </c>
       <c r="AA64" t="s" s="2">
-        <v>289</v>
-      </c>
-      <c r="AB64" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="AB64" t="s" s="2">
+        <v>38</v>
+      </c>
       <c r="AC64" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AD64" t="s" s="2">
-        <v>290</v>
+        <v>38</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>269</v>
+        <v>284</v>
       </c>
       <c r="AF64" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="AG64" t="s" s="2">
         <v>47</v>
@@ -8005,7 +8021,7 @@
         <v>59</v>
       </c>
       <c r="AJ64" t="s" s="2">
-        <v>276</v>
+        <v>38</v>
       </c>
       <c r="AK64" t="s" s="2">
         <v>38</v>
@@ -8013,17 +8029,17 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>269</v>
+        <v>247</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>291</v>
+        <v>302</v>
       </c>
       <c r="C65" t="s" s="2">
         <v>38</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F65" t="s" s="2">
         <v>47</v>
@@ -8038,19 +8054,19 @@
         <v>38</v>
       </c>
       <c r="J65" t="s" s="2">
-        <v>138</v>
+        <v>249</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>271</v>
+        <v>303</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>272</v>
+        <v>251</v>
       </c>
       <c r="M65" t="s" s="2">
-        <v>273</v>
+        <v>304</v>
       </c>
       <c r="N65" t="s" s="2">
-        <v>274</v>
+        <v>253</v>
       </c>
       <c r="O65" t="s" s="2">
         <v>38</v>
@@ -8075,11 +8091,13 @@
         <v>38</v>
       </c>
       <c r="W65" t="s" s="2">
-        <v>185</v>
-      </c>
-      <c r="X65" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="X65" t="s" s="2">
+        <v>38</v>
+      </c>
       <c r="Y65" t="s" s="2">
-        <v>298</v>
+        <v>38</v>
       </c>
       <c r="Z65" t="s" s="2">
         <v>38</v>
@@ -8097,13 +8115,13 @@
         <v>38</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>269</v>
+        <v>247</v>
       </c>
       <c r="AF65" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="AG65" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AH65" t="s" s="2">
         <v>38</v>
@@ -8112,7 +8130,7 @@
         <v>59</v>
       </c>
       <c r="AJ65" t="s" s="2">
-        <v>276</v>
+        <v>256</v>
       </c>
       <c r="AK65" t="s" s="2">
         <v>38</v>
@@ -8120,7 +8138,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>277</v>
+        <v>257</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -8128,7 +8146,7 @@
       </c>
       <c r="D66" s="2"/>
       <c r="E66" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F66" t="s" s="2">
         <v>47</v>
@@ -8143,20 +8161,16 @@
         <v>38</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>112</v>
+        <v>49</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>278</v>
+        <v>165</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>279</v>
-      </c>
-      <c r="M66" t="s" s="2">
-        <v>280</v>
-      </c>
-      <c r="N66" t="s" s="2">
-        <v>281</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="M66" s="2"/>
+      <c r="N66" s="2"/>
       <c r="O66" t="s" s="2">
         <v>38</v>
       </c>
@@ -8204,10 +8218,10 @@
         <v>38</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>277</v>
+        <v>167</v>
       </c>
       <c r="AF66" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="AG66" t="s" s="2">
         <v>47</v>
@@ -8216,10 +8230,10 @@
         <v>38</v>
       </c>
       <c r="AI66" t="s" s="2">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="AJ66" t="s" s="2">
-        <v>283</v>
+        <v>168</v>
       </c>
       <c r="AK66" t="s" s="2">
         <v>38</v>
@@ -8227,18 +8241,18 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>284</v>
+        <v>258</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F67" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G67" t="s" s="2">
         <v>38</v>
@@ -8250,15 +8264,17 @@
         <v>38</v>
       </c>
       <c r="J67" t="s" s="2">
-        <v>231</v>
+        <v>93</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>285</v>
+        <v>94</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>286</v>
-      </c>
-      <c r="M67" s="2"/>
+        <v>170</v>
+      </c>
+      <c r="M67" t="s" s="2">
+        <v>96</v>
+      </c>
       <c r="N67" s="2"/>
       <c r="O67" t="s" s="2">
         <v>38</v>
@@ -8307,22 +8323,22 @@
         <v>38</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>284</v>
+        <v>174</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG67" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AH67" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AI67" t="s" s="2">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="AJ67" t="s" s="2">
-        <v>38</v>
+        <v>168</v>
       </c>
       <c r="AK67" t="s" s="2">
         <v>38</v>
@@ -8330,44 +8346,42 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>247</v>
-      </c>
-      <c r="B68" t="s" s="2">
-        <v>299</v>
-      </c>
+        <v>259</v>
+      </c>
+      <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
-        <v>38</v>
+        <v>260</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F68" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G68" t="s" s="2">
         <v>38</v>
       </c>
       <c r="H68" t="s" s="2">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="I68" t="s" s="2">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="J68" t="s" s="2">
-        <v>249</v>
+        <v>93</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>251</v>
+        <v>262</v>
       </c>
       <c r="M68" t="s" s="2">
-        <v>252</v>
+        <v>96</v>
       </c>
       <c r="N68" t="s" s="2">
-        <v>253</v>
+        <v>102</v>
       </c>
       <c r="O68" t="s" s="2">
         <v>38</v>
@@ -8416,7 +8430,7 @@
         <v>38</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>247</v>
+        <v>263</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>39</v>
@@ -8428,10 +8442,10 @@
         <v>38</v>
       </c>
       <c r="AI68" t="s" s="2">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="AJ68" t="s" s="2">
-        <v>256</v>
+        <v>90</v>
       </c>
       <c r="AK68" t="s" s="2">
         <v>38</v>
@@ -8439,7 +8453,7 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -8447,7 +8461,7 @@
       </c>
       <c r="D69" s="2"/>
       <c r="E69" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F69" t="s" s="2">
         <v>47</v>
@@ -8462,16 +8476,18 @@
         <v>38</v>
       </c>
       <c r="J69" t="s" s="2">
-        <v>49</v>
+        <v>138</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>165</v>
+        <v>265</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>166</v>
+        <v>266</v>
       </c>
       <c r="M69" s="2"/>
-      <c r="N69" s="2"/>
+      <c r="N69" t="s" s="2">
+        <v>267</v>
+      </c>
       <c r="O69" t="s" s="2">
         <v>38</v>
       </c>
@@ -8480,7 +8496,7 @@
         <v>38</v>
       </c>
       <c r="R69" t="s" s="2">
-        <v>38</v>
+        <v>305</v>
       </c>
       <c r="S69" t="s" s="2">
         <v>38</v>
@@ -8495,10 +8511,10 @@
         <v>38</v>
       </c>
       <c r="W69" t="s" s="2">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="X69" t="s" s="2">
-        <v>38</v>
+        <v>268</v>
       </c>
       <c r="Y69" t="s" s="2">
         <v>38</v>
@@ -8519,10 +8535,10 @@
         <v>38</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>167</v>
+        <v>264</v>
       </c>
       <c r="AF69" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="AG69" t="s" s="2">
         <v>47</v>
@@ -8531,10 +8547,10 @@
         <v>38</v>
       </c>
       <c r="AI69" t="s" s="2">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="AJ69" t="s" s="2">
-        <v>168</v>
+        <v>145</v>
       </c>
       <c r="AK69" t="s" s="2">
         <v>38</v>
@@ -8542,18 +8558,18 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>258</v>
+        <v>269</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
-        <v>92</v>
+        <v>38</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F70" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="G70" t="s" s="2">
         <v>38</v>
@@ -8565,18 +8581,20 @@
         <v>38</v>
       </c>
       <c r="J70" t="s" s="2">
-        <v>93</v>
+        <v>138</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>94</v>
+        <v>271</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>170</v>
+        <v>272</v>
       </c>
       <c r="M70" t="s" s="2">
-        <v>96</v>
-      </c>
-      <c r="N70" s="2"/>
+        <v>273</v>
+      </c>
+      <c r="N70" t="s" s="2">
+        <v>274</v>
+      </c>
       <c r="O70" t="s" s="2">
         <v>38</v>
       </c>
@@ -8600,13 +8618,11 @@
         <v>38</v>
       </c>
       <c r="W70" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="X70" t="s" s="2">
-        <v>38</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="X70" s="2"/>
       <c r="Y70" t="s" s="2">
-        <v>38</v>
+        <v>306</v>
       </c>
       <c r="Z70" t="s" s="2">
         <v>38</v>
@@ -8624,22 +8640,22 @@
         <v>38</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>174</v>
+        <v>269</v>
       </c>
       <c r="AF70" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="AG70" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="AH70" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AI70" t="s" s="2">
-        <v>98</v>
+        <v>59</v>
       </c>
       <c r="AJ70" t="s" s="2">
-        <v>168</v>
+        <v>276</v>
       </c>
       <c r="AK70" t="s" s="2">
         <v>38</v>
@@ -8647,42 +8663,42 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>259</v>
+        <v>277</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
-        <v>260</v>
+        <v>38</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F71" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="G71" t="s" s="2">
         <v>38</v>
       </c>
       <c r="H71" t="s" s="2">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="I71" t="s" s="2">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="J71" t="s" s="2">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="K71" t="s" s="2">
-        <v>261</v>
+        <v>278</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>262</v>
+        <v>279</v>
       </c>
       <c r="M71" t="s" s="2">
-        <v>96</v>
+        <v>280</v>
       </c>
       <c r="N71" t="s" s="2">
-        <v>102</v>
+        <v>281</v>
       </c>
       <c r="O71" t="s" s="2">
         <v>38</v>
@@ -8731,22 +8747,22 @@
         <v>38</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>263</v>
+        <v>277</v>
       </c>
       <c r="AF71" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="AG71" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="AH71" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AI71" t="s" s="2">
-        <v>98</v>
+        <v>59</v>
       </c>
       <c r="AJ71" t="s" s="2">
-        <v>90</v>
+        <v>283</v>
       </c>
       <c r="AK71" t="s" s="2">
         <v>38</v>
@@ -8754,7 +8770,7 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>264</v>
+        <v>284</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -8762,7 +8778,7 @@
       </c>
       <c r="D72" s="2"/>
       <c r="E72" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F72" t="s" s="2">
         <v>47</v>
@@ -8777,18 +8793,16 @@
         <v>38</v>
       </c>
       <c r="J72" t="s" s="2">
-        <v>138</v>
+        <v>231</v>
       </c>
       <c r="K72" t="s" s="2">
-        <v>265</v>
+        <v>285</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>266</v>
+        <v>286</v>
       </c>
       <c r="M72" s="2"/>
-      <c r="N72" t="s" s="2">
-        <v>267</v>
-      </c>
+      <c r="N72" s="2"/>
       <c r="O72" t="s" s="2">
         <v>38</v>
       </c>
@@ -8797,7 +8811,7 @@
         <v>38</v>
       </c>
       <c r="R72" t="s" s="2">
-        <v>300</v>
+        <v>38</v>
       </c>
       <c r="S72" t="s" s="2">
         <v>38</v>
@@ -8812,10 +8826,10 @@
         <v>38</v>
       </c>
       <c r="W72" t="s" s="2">
-        <v>143</v>
+        <v>38</v>
       </c>
       <c r="X72" t="s" s="2">
-        <v>268</v>
+        <v>38</v>
       </c>
       <c r="Y72" t="s" s="2">
         <v>38</v>
@@ -8836,10 +8850,10 @@
         <v>38</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>264</v>
+        <v>284</v>
       </c>
       <c r="AF72" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="AG72" t="s" s="2">
         <v>47</v>
@@ -8851,7 +8865,7 @@
         <v>59</v>
       </c>
       <c r="AJ72" t="s" s="2">
-        <v>145</v>
+        <v>38</v>
       </c>
       <c r="AK72" t="s" s="2">
         <v>38</v>
@@ -8859,9 +8873,11 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="B73" s="2"/>
+        <v>247</v>
+      </c>
+      <c r="B73" t="s" s="2">
+        <v>307</v>
+      </c>
       <c r="C73" t="s" s="2">
         <v>38</v>
       </c>
@@ -8882,19 +8898,19 @@
         <v>38</v>
       </c>
       <c r="J73" t="s" s="2">
-        <v>138</v>
+        <v>249</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>271</v>
+        <v>308</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>272</v>
+        <v>251</v>
       </c>
       <c r="M73" t="s" s="2">
-        <v>273</v>
+        <v>309</v>
       </c>
       <c r="N73" t="s" s="2">
-        <v>274</v>
+        <v>253</v>
       </c>
       <c r="O73" t="s" s="2">
         <v>38</v>
@@ -8919,10 +8935,10 @@
         <v>38</v>
       </c>
       <c r="W73" t="s" s="2">
-        <v>143</v>
+        <v>38</v>
       </c>
       <c r="X73" t="s" s="2">
-        <v>275</v>
+        <v>38</v>
       </c>
       <c r="Y73" t="s" s="2">
         <v>38</v>
@@ -8931,23 +8947,25 @@
         <v>38</v>
       </c>
       <c r="AA73" t="s" s="2">
-        <v>289</v>
-      </c>
-      <c r="AB73" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="AB73" t="s" s="2">
+        <v>38</v>
+      </c>
       <c r="AC73" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AD73" t="s" s="2">
-        <v>290</v>
+        <v>38</v>
       </c>
       <c r="AE73" t="s" s="2">
-        <v>269</v>
+        <v>247</v>
       </c>
       <c r="AF73" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="AG73" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AH73" t="s" s="2">
         <v>38</v>
@@ -8956,7 +8974,7 @@
         <v>59</v>
       </c>
       <c r="AJ73" t="s" s="2">
-        <v>276</v>
+        <v>256</v>
       </c>
       <c r="AK73" t="s" s="2">
         <v>38</v>
@@ -8964,11 +8982,9 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="B74" t="s" s="2">
-        <v>291</v>
-      </c>
+        <v>257</v>
+      </c>
+      <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
         <v>38</v>
       </c>
@@ -8989,20 +9005,16 @@
         <v>38</v>
       </c>
       <c r="J74" t="s" s="2">
-        <v>138</v>
+        <v>49</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>271</v>
+        <v>165</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>272</v>
-      </c>
-      <c r="M74" t="s" s="2">
-        <v>273</v>
-      </c>
-      <c r="N74" t="s" s="2">
-        <v>274</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="M74" s="2"/>
+      <c r="N74" s="2"/>
       <c r="O74" t="s" s="2">
         <v>38</v>
       </c>
@@ -9026,11 +9038,13 @@
         <v>38</v>
       </c>
       <c r="W74" t="s" s="2">
-        <v>125</v>
-      </c>
-      <c r="X74" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="X74" t="s" s="2">
+        <v>38</v>
+      </c>
       <c r="Y74" t="s" s="2">
-        <v>301</v>
+        <v>38</v>
       </c>
       <c r="Z74" t="s" s="2">
         <v>38</v>
@@ -9048,10 +9062,10 @@
         <v>38</v>
       </c>
       <c r="AE74" t="s" s="2">
-        <v>269</v>
+        <v>167</v>
       </c>
       <c r="AF74" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="AG74" t="s" s="2">
         <v>47</v>
@@ -9060,10 +9074,10 @@
         <v>38</v>
       </c>
       <c r="AI74" t="s" s="2">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="AJ74" t="s" s="2">
-        <v>276</v>
+        <v>168</v>
       </c>
       <c r="AK74" t="s" s="2">
         <v>38</v>
@@ -9071,18 +9085,18 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>277</v>
+        <v>258</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F75" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G75" t="s" s="2">
         <v>38</v>
@@ -9094,20 +9108,18 @@
         <v>38</v>
       </c>
       <c r="J75" t="s" s="2">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="K75" t="s" s="2">
-        <v>278</v>
+        <v>94</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>279</v>
+        <v>170</v>
       </c>
       <c r="M75" t="s" s="2">
-        <v>280</v>
-      </c>
-      <c r="N75" t="s" s="2">
-        <v>281</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="N75" s="2"/>
       <c r="O75" t="s" s="2">
         <v>38</v>
       </c>
@@ -9155,22 +9167,22 @@
         <v>38</v>
       </c>
       <c r="AE75" t="s" s="2">
-        <v>277</v>
+        <v>174</v>
       </c>
       <c r="AF75" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="AG75" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AH75" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AI75" t="s" s="2">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="AJ75" t="s" s="2">
-        <v>283</v>
+        <v>168</v>
       </c>
       <c r="AK75" t="s" s="2">
         <v>38</v>
@@ -9178,39 +9190,43 @@
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>284</v>
+        <v>259</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
-        <v>38</v>
+        <v>260</v>
       </c>
       <c r="D76" s="2"/>
       <c r="E76" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F76" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G76" t="s" s="2">
         <v>38</v>
       </c>
       <c r="H76" t="s" s="2">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="I76" t="s" s="2">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="J76" t="s" s="2">
-        <v>231</v>
+        <v>93</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>285</v>
+        <v>261</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>286</v>
-      </c>
-      <c r="M76" s="2"/>
-      <c r="N76" s="2"/>
+        <v>262</v>
+      </c>
+      <c r="M76" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="N76" t="s" s="2">
+        <v>102</v>
+      </c>
       <c r="O76" t="s" s="2">
         <v>38</v>
       </c>
@@ -9258,22 +9274,22 @@
         <v>38</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>284</v>
+        <v>263</v>
       </c>
       <c r="AF76" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG76" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AH76" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AI76" t="s" s="2">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="AJ76" t="s" s="2">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="AK76" t="s" s="2">
         <v>38</v>
@@ -9281,11 +9297,9 @@
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>247</v>
-      </c>
-      <c r="B77" t="s" s="2">
-        <v>302</v>
-      </c>
+        <v>264</v>
+      </c>
+      <c r="B77" s="2"/>
       <c r="C77" t="s" s="2">
         <v>38</v>
       </c>
@@ -9306,19 +9320,17 @@
         <v>38</v>
       </c>
       <c r="J77" t="s" s="2">
-        <v>249</v>
+        <v>138</v>
       </c>
       <c r="K77" t="s" s="2">
-        <v>250</v>
+        <v>265</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>251</v>
-      </c>
-      <c r="M77" t="s" s="2">
-        <v>252</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="M77" s="2"/>
       <c r="N77" t="s" s="2">
-        <v>253</v>
+        <v>267</v>
       </c>
       <c r="O77" t="s" s="2">
         <v>38</v>
@@ -9328,7 +9340,7 @@
         <v>38</v>
       </c>
       <c r="R77" t="s" s="2">
-        <v>38</v>
+        <v>310</v>
       </c>
       <c r="S77" t="s" s="2">
         <v>38</v>
@@ -9343,10 +9355,10 @@
         <v>38</v>
       </c>
       <c r="W77" t="s" s="2">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="X77" t="s" s="2">
-        <v>38</v>
+        <v>268</v>
       </c>
       <c r="Y77" t="s" s="2">
         <v>38</v>
@@ -9367,13 +9379,13 @@
         <v>38</v>
       </c>
       <c r="AE77" t="s" s="2">
-        <v>247</v>
+        <v>264</v>
       </c>
       <c r="AF77" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="AG77" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="AH77" t="s" s="2">
         <v>38</v>
@@ -9382,7 +9394,7 @@
         <v>59</v>
       </c>
       <c r="AJ77" t="s" s="2">
-        <v>256</v>
+        <v>145</v>
       </c>
       <c r="AK77" t="s" s="2">
         <v>38</v>
@@ -9390,7 +9402,7 @@
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>257</v>
+        <v>269</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
@@ -9398,7 +9410,7 @@
       </c>
       <c r="D78" s="2"/>
       <c r="E78" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F78" t="s" s="2">
         <v>47</v>
@@ -9413,16 +9425,20 @@
         <v>38</v>
       </c>
       <c r="J78" t="s" s="2">
-        <v>49</v>
+        <v>311</v>
       </c>
       <c r="K78" t="s" s="2">
-        <v>165</v>
+        <v>271</v>
       </c>
       <c r="L78" t="s" s="2">
-        <v>166</v>
-      </c>
-      <c r="M78" s="2"/>
-      <c r="N78" s="2"/>
+        <v>272</v>
+      </c>
+      <c r="M78" t="s" s="2">
+        <v>273</v>
+      </c>
+      <c r="N78" t="s" s="2">
+        <v>274</v>
+      </c>
       <c r="O78" t="s" s="2">
         <v>38</v>
       </c>
@@ -9470,10 +9486,10 @@
         <v>38</v>
       </c>
       <c r="AE78" t="s" s="2">
-        <v>167</v>
+        <v>269</v>
       </c>
       <c r="AF78" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="AG78" t="s" s="2">
         <v>47</v>
@@ -9482,10 +9498,10 @@
         <v>38</v>
       </c>
       <c r="AI78" t="s" s="2">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="AJ78" t="s" s="2">
-        <v>168</v>
+        <v>276</v>
       </c>
       <c r="AK78" t="s" s="2">
         <v>38</v>
@@ -9493,18 +9509,18 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>258</v>
+        <v>277</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
-        <v>92</v>
+        <v>38</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F79" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="G79" t="s" s="2">
         <v>38</v>
@@ -9516,18 +9532,20 @@
         <v>38</v>
       </c>
       <c r="J79" t="s" s="2">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="K79" t="s" s="2">
-        <v>94</v>
+        <v>278</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>170</v>
+        <v>279</v>
       </c>
       <c r="M79" t="s" s="2">
-        <v>96</v>
-      </c>
-      <c r="N79" s="2"/>
+        <v>280</v>
+      </c>
+      <c r="N79" t="s" s="2">
+        <v>281</v>
+      </c>
       <c r="O79" t="s" s="2">
         <v>38</v>
       </c>
@@ -9575,22 +9593,22 @@
         <v>38</v>
       </c>
       <c r="AE79" t="s" s="2">
-        <v>174</v>
+        <v>277</v>
       </c>
       <c r="AF79" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="AG79" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="AH79" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AI79" t="s" s="2">
-        <v>98</v>
+        <v>59</v>
       </c>
       <c r="AJ79" t="s" s="2">
-        <v>168</v>
+        <v>283</v>
       </c>
       <c r="AK79" t="s" s="2">
         <v>38</v>
@@ -9598,43 +9616,39 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>259</v>
+        <v>284</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
-        <v>260</v>
+        <v>38</v>
       </c>
       <c r="D80" s="2"/>
       <c r="E80" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F80" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="G80" t="s" s="2">
         <v>38</v>
       </c>
       <c r="H80" t="s" s="2">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="I80" t="s" s="2">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="J80" t="s" s="2">
-        <v>93</v>
+        <v>231</v>
       </c>
       <c r="K80" t="s" s="2">
-        <v>261</v>
+        <v>285</v>
       </c>
       <c r="L80" t="s" s="2">
-        <v>262</v>
-      </c>
-      <c r="M80" t="s" s="2">
-        <v>96</v>
-      </c>
-      <c r="N80" t="s" s="2">
-        <v>102</v>
-      </c>
+        <v>286</v>
+      </c>
+      <c r="M80" s="2"/>
+      <c r="N80" s="2"/>
       <c r="O80" t="s" s="2">
         <v>38</v>
       </c>
@@ -9682,22 +9696,22 @@
         <v>38</v>
       </c>
       <c r="AE80" t="s" s="2">
-        <v>263</v>
+        <v>284</v>
       </c>
       <c r="AF80" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG80" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="AH80" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AI80" t="s" s="2">
-        <v>98</v>
+        <v>59</v>
       </c>
       <c r="AJ80" t="s" s="2">
-        <v>90</v>
+        <v>38</v>
       </c>
       <c r="AK80" t="s" s="2">
         <v>38</v>
@@ -9705,7 +9719,7 @@
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
-        <v>264</v>
+        <v>312</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" t="s" s="2">
@@ -9713,10 +9727,10 @@
       </c>
       <c r="D81" s="2"/>
       <c r="E81" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F81" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G81" t="s" s="2">
         <v>38</v>
@@ -9728,17 +9742,17 @@
         <v>38</v>
       </c>
       <c r="J81" t="s" s="2">
-        <v>138</v>
+        <v>249</v>
       </c>
       <c r="K81" t="s" s="2">
-        <v>265</v>
+        <v>313</v>
       </c>
       <c r="L81" t="s" s="2">
-        <v>266</v>
+        <v>314</v>
       </c>
       <c r="M81" s="2"/>
       <c r="N81" t="s" s="2">
-        <v>267</v>
+        <v>315</v>
       </c>
       <c r="O81" t="s" s="2">
         <v>38</v>
@@ -9748,7 +9762,7 @@
         <v>38</v>
       </c>
       <c r="R81" t="s" s="2">
-        <v>303</v>
+        <v>38</v>
       </c>
       <c r="S81" t="s" s="2">
         <v>38</v>
@@ -9763,10 +9777,10 @@
         <v>38</v>
       </c>
       <c r="W81" t="s" s="2">
-        <v>143</v>
+        <v>38</v>
       </c>
       <c r="X81" t="s" s="2">
-        <v>268</v>
+        <v>38</v>
       </c>
       <c r="Y81" t="s" s="2">
         <v>38</v>
@@ -9787,22 +9801,22 @@
         <v>38</v>
       </c>
       <c r="AE81" t="s" s="2">
-        <v>264</v>
+        <v>312</v>
       </c>
       <c r="AF81" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="AG81" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AH81" t="s" s="2">
-        <v>38</v>
+        <v>135</v>
       </c>
       <c r="AI81" t="s" s="2">
         <v>59</v>
       </c>
       <c r="AJ81" t="s" s="2">
-        <v>145</v>
+        <v>316</v>
       </c>
       <c r="AK81" t="s" s="2">
         <v>38</v>
@@ -9810,7 +9824,7 @@
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>269</v>
+        <v>317</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" t="s" s="2">
@@ -9818,7 +9832,7 @@
       </c>
       <c r="D82" s="2"/>
       <c r="E82" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F82" t="s" s="2">
         <v>47</v>
@@ -9833,20 +9847,16 @@
         <v>38</v>
       </c>
       <c r="J82" t="s" s="2">
-        <v>304</v>
+        <v>49</v>
       </c>
       <c r="K82" t="s" s="2">
-        <v>271</v>
+        <v>165</v>
       </c>
       <c r="L82" t="s" s="2">
-        <v>272</v>
-      </c>
-      <c r="M82" t="s" s="2">
-        <v>273</v>
-      </c>
-      <c r="N82" t="s" s="2">
-        <v>274</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="M82" s="2"/>
+      <c r="N82" s="2"/>
       <c r="O82" t="s" s="2">
         <v>38</v>
       </c>
@@ -9894,10 +9904,10 @@
         <v>38</v>
       </c>
       <c r="AE82" t="s" s="2">
-        <v>269</v>
+        <v>167</v>
       </c>
       <c r="AF82" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="AG82" t="s" s="2">
         <v>47</v>
@@ -9906,10 +9916,10 @@
         <v>38</v>
       </c>
       <c r="AI82" t="s" s="2">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="AJ82" t="s" s="2">
-        <v>276</v>
+        <v>168</v>
       </c>
       <c r="AK82" t="s" s="2">
         <v>38</v>
@@ -9917,18 +9927,18 @@
     </row>
     <row r="83" hidden="true">
       <c r="A83" t="s" s="2">
-        <v>277</v>
+        <v>318</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" t="s" s="2">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F83" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G83" t="s" s="2">
         <v>38</v>
@@ -9940,20 +9950,18 @@
         <v>38</v>
       </c>
       <c r="J83" t="s" s="2">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="K83" t="s" s="2">
-        <v>278</v>
+        <v>94</v>
       </c>
       <c r="L83" t="s" s="2">
-        <v>279</v>
+        <v>170</v>
       </c>
       <c r="M83" t="s" s="2">
-        <v>280</v>
-      </c>
-      <c r="N83" t="s" s="2">
-        <v>281</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="N83" s="2"/>
       <c r="O83" t="s" s="2">
         <v>38</v>
       </c>
@@ -10001,22 +10009,22 @@
         <v>38</v>
       </c>
       <c r="AE83" t="s" s="2">
-        <v>277</v>
+        <v>174</v>
       </c>
       <c r="AF83" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="AG83" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AH83" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AI83" t="s" s="2">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="AJ83" t="s" s="2">
-        <v>283</v>
+        <v>168</v>
       </c>
       <c r="AK83" t="s" s="2">
         <v>38</v>
@@ -10024,39 +10032,43 @@
     </row>
     <row r="84" hidden="true">
       <c r="A84" t="s" s="2">
-        <v>284</v>
+        <v>319</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" t="s" s="2">
-        <v>38</v>
+        <v>260</v>
       </c>
       <c r="D84" s="2"/>
       <c r="E84" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F84" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G84" t="s" s="2">
         <v>38</v>
       </c>
       <c r="H84" t="s" s="2">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="I84" t="s" s="2">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="J84" t="s" s="2">
-        <v>231</v>
+        <v>93</v>
       </c>
       <c r="K84" t="s" s="2">
-        <v>285</v>
+        <v>261</v>
       </c>
       <c r="L84" t="s" s="2">
-        <v>286</v>
-      </c>
-      <c r="M84" s="2"/>
-      <c r="N84" s="2"/>
+        <v>262</v>
+      </c>
+      <c r="M84" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="N84" t="s" s="2">
+        <v>102</v>
+      </c>
       <c r="O84" t="s" s="2">
         <v>38</v>
       </c>
@@ -10104,22 +10116,22 @@
         <v>38</v>
       </c>
       <c r="AE84" t="s" s="2">
-        <v>284</v>
+        <v>263</v>
       </c>
       <c r="AF84" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG84" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AH84" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AI84" t="s" s="2">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="AJ84" t="s" s="2">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="AK84" t="s" s="2">
         <v>38</v>
@@ -10127,7 +10139,7 @@
     </row>
     <row r="85" hidden="true">
       <c r="A85" t="s" s="2">
-        <v>305</v>
+        <v>320</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" t="s" s="2">
@@ -10135,10 +10147,10 @@
       </c>
       <c r="D85" s="2"/>
       <c r="E85" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F85" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="G85" t="s" s="2">
         <v>38</v>
@@ -10150,18 +10162,16 @@
         <v>38</v>
       </c>
       <c r="J85" t="s" s="2">
-        <v>249</v>
+        <v>321</v>
       </c>
       <c r="K85" t="s" s="2">
-        <v>306</v>
+        <v>322</v>
       </c>
       <c r="L85" t="s" s="2">
-        <v>307</v>
+        <v>323</v>
       </c>
       <c r="M85" s="2"/>
-      <c r="N85" t="s" s="2">
-        <v>308</v>
-      </c>
+      <c r="N85" s="2"/>
       <c r="O85" t="s" s="2">
         <v>38</v>
       </c>
@@ -10209,22 +10219,22 @@
         <v>38</v>
       </c>
       <c r="AE85" t="s" s="2">
-        <v>305</v>
+        <v>320</v>
       </c>
       <c r="AF85" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="AG85" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="AH85" t="s" s="2">
-        <v>135</v>
+        <v>38</v>
       </c>
       <c r="AI85" t="s" s="2">
         <v>59</v>
       </c>
       <c r="AJ85" t="s" s="2">
-        <v>309</v>
+        <v>38</v>
       </c>
       <c r="AK85" t="s" s="2">
         <v>38</v>
@@ -10232,7 +10242,7 @@
     </row>
     <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
-        <v>310</v>
+        <v>324</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" t="s" s="2">
@@ -10255,20 +10265,24 @@
         <v>38</v>
       </c>
       <c r="J86" t="s" s="2">
-        <v>49</v>
+        <v>231</v>
       </c>
       <c r="K86" t="s" s="2">
-        <v>165</v>
+        <v>325</v>
       </c>
       <c r="L86" t="s" s="2">
-        <v>166</v>
+        <v>326</v>
       </c>
       <c r="M86" s="2"/>
-      <c r="N86" s="2"/>
+      <c r="N86" t="s" s="2">
+        <v>327</v>
+      </c>
       <c r="O86" t="s" s="2">
         <v>38</v>
       </c>
-      <c r="P86" s="2"/>
+      <c r="P86" t="s" s="2">
+        <v>328</v>
+      </c>
       <c r="Q86" t="s" s="2">
         <v>38</v>
       </c>
@@ -10312,7 +10326,7 @@
         <v>38</v>
       </c>
       <c r="AE86" t="s" s="2">
-        <v>167</v>
+        <v>324</v>
       </c>
       <c r="AF86" t="s" s="2">
         <v>39</v>
@@ -10324,10 +10338,10 @@
         <v>38</v>
       </c>
       <c r="AI86" t="s" s="2">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="AJ86" t="s" s="2">
-        <v>168</v>
+        <v>38</v>
       </c>
       <c r="AK86" t="s" s="2">
         <v>38</v>
@@ -10335,18 +10349,18 @@
     </row>
     <row r="87" hidden="true">
       <c r="A87" t="s" s="2">
-        <v>311</v>
+        <v>329</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" t="s" s="2">
-        <v>92</v>
+        <v>38</v>
       </c>
       <c r="D87" s="2"/>
       <c r="E87" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F87" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="G87" t="s" s="2">
         <v>38</v>
@@ -10358,22 +10372,24 @@
         <v>38</v>
       </c>
       <c r="J87" t="s" s="2">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="K87" t="s" s="2">
-        <v>94</v>
+        <v>330</v>
       </c>
       <c r="L87" t="s" s="2">
-        <v>170</v>
-      </c>
-      <c r="M87" t="s" s="2">
-        <v>96</v>
-      </c>
-      <c r="N87" s="2"/>
+        <v>331</v>
+      </c>
+      <c r="M87" s="2"/>
+      <c r="N87" t="s" s="2">
+        <v>332</v>
+      </c>
       <c r="O87" t="s" s="2">
         <v>38</v>
       </c>
-      <c r="P87" s="2"/>
+      <c r="P87" t="s" s="2">
+        <v>333</v>
+      </c>
       <c r="Q87" t="s" s="2">
         <v>38</v>
       </c>
@@ -10417,453 +10433,29 @@
         <v>38</v>
       </c>
       <c r="AE87" t="s" s="2">
-        <v>174</v>
+        <v>329</v>
       </c>
       <c r="AF87" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG87" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="AH87" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AI87" t="s" s="2">
-        <v>98</v>
+        <v>59</v>
       </c>
       <c r="AJ87" t="s" s="2">
-        <v>168</v>
+        <v>38</v>
       </c>
       <c r="AK87" t="s" s="2">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="88" hidden="true">
-      <c r="A88" t="s" s="2">
-        <v>312</v>
-      </c>
-      <c r="B88" s="2"/>
-      <c r="C88" t="s" s="2">
-        <v>260</v>
-      </c>
-      <c r="D88" s="2"/>
-      <c r="E88" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F88" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="G88" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="H88" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="I88" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="J88" t="s" s="2">
-        <v>93</v>
-      </c>
-      <c r="K88" t="s" s="2">
-        <v>261</v>
-      </c>
-      <c r="L88" t="s" s="2">
-        <v>262</v>
-      </c>
-      <c r="M88" t="s" s="2">
-        <v>96</v>
-      </c>
-      <c r="N88" t="s" s="2">
-        <v>102</v>
-      </c>
-      <c r="O88" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="P88" s="2"/>
-      <c r="Q88" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="R88" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="S88" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="T88" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="U88" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="V88" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="W88" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="X88" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Y88" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Z88" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AA88" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AB88" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AC88" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AD88" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AE88" t="s" s="2">
-        <v>263</v>
-      </c>
-      <c r="AF88" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG88" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AH88" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AI88" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="AJ88" t="s" s="2">
-        <v>90</v>
-      </c>
-      <c r="AK88" t="s" s="2">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="89" hidden="true">
-      <c r="A89" t="s" s="2">
-        <v>313</v>
-      </c>
-      <c r="B89" s="2"/>
-      <c r="C89" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="D89" s="2"/>
-      <c r="E89" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="F89" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="G89" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="H89" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="I89" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="J89" t="s" s="2">
-        <v>314</v>
-      </c>
-      <c r="K89" t="s" s="2">
-        <v>315</v>
-      </c>
-      <c r="L89" t="s" s="2">
-        <v>316</v>
-      </c>
-      <c r="M89" s="2"/>
-      <c r="N89" s="2"/>
-      <c r="O89" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="P89" s="2"/>
-      <c r="Q89" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="R89" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="S89" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="T89" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="U89" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="V89" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="W89" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="X89" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Y89" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Z89" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AA89" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AB89" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AC89" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AD89" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AE89" t="s" s="2">
-        <v>313</v>
-      </c>
-      <c r="AF89" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="AG89" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="AH89" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AI89" t="s" s="2">
-        <v>59</v>
-      </c>
-      <c r="AJ89" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AK89" t="s" s="2">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="90" hidden="true">
-      <c r="A90" t="s" s="2">
-        <v>317</v>
-      </c>
-      <c r="B90" s="2"/>
-      <c r="C90" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="D90" s="2"/>
-      <c r="E90" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F90" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="G90" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="H90" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="I90" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="J90" t="s" s="2">
-        <v>231</v>
-      </c>
-      <c r="K90" t="s" s="2">
-        <v>318</v>
-      </c>
-      <c r="L90" t="s" s="2">
-        <v>319</v>
-      </c>
-      <c r="M90" s="2"/>
-      <c r="N90" t="s" s="2">
-        <v>320</v>
-      </c>
-      <c r="O90" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="P90" t="s" s="2">
-        <v>321</v>
-      </c>
-      <c r="Q90" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="R90" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="S90" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="T90" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="U90" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="V90" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="W90" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="X90" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Y90" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Z90" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AA90" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AB90" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AC90" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AD90" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AE90" t="s" s="2">
-        <v>317</v>
-      </c>
-      <c r="AF90" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG90" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="AH90" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AI90" t="s" s="2">
-        <v>59</v>
-      </c>
-      <c r="AJ90" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AK90" t="s" s="2">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="91" hidden="true">
-      <c r="A91" t="s" s="2">
-        <v>322</v>
-      </c>
-      <c r="B91" s="2"/>
-      <c r="C91" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="D91" s="2"/>
-      <c r="E91" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F91" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="G91" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="H91" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="I91" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="J91" t="s" s="2">
-        <v>112</v>
-      </c>
-      <c r="K91" t="s" s="2">
-        <v>323</v>
-      </c>
-      <c r="L91" t="s" s="2">
-        <v>324</v>
-      </c>
-      <c r="M91" s="2"/>
-      <c r="N91" t="s" s="2">
-        <v>325</v>
-      </c>
-      <c r="O91" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="P91" t="s" s="2">
-        <v>326</v>
-      </c>
-      <c r="Q91" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="R91" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="S91" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="T91" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="U91" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="V91" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="W91" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="X91" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Y91" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="Z91" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AA91" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AB91" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AC91" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AD91" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AE91" t="s" s="2">
-        <v>322</v>
-      </c>
-      <c r="AF91" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG91" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="AH91" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AI91" t="s" s="2">
-        <v>59</v>
-      </c>
-      <c r="AJ91" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="AK91" t="s" s="2">
         <v>38</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AK91">
+  <autoFilter ref="A1:AK87">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -10873,7 +10465,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI90">
+  <conditionalFormatting sqref="A2:AI86">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Reworked actors and transactions to support MeasureReport.
Added new Profiles (empty) to support MeasureReport.

Closes #32
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-saner-bed-group.xlsx
+++ b/docs/StructureDefinition-saner-bed-group.xlsx
@@ -900,9 +900,6 @@
     <t>Sometimes group membership is determined by characteristics not possessed.</t>
   </si>
   <si>
-    <t>false</t>
-  </si>
-  <si>
     <t>./valueNegationInd</t>
   </si>
   <si>
@@ -933,6 +930,9 @@
   </si>
   <si>
     <t>http://hl7.org/fhir/ValueSet/location-status</t>
+  </si>
+  <si>
+    <t>false</t>
   </si>
   <si>
     <t>OperationalStatus</t>
@@ -5329,7 +5329,7 @@
       </c>
       <c r="P39" s="2"/>
       <c r="Q39" t="s" s="2">
-        <v>282</v>
+        <v>38</v>
       </c>
       <c r="R39" t="s" s="2">
         <v>38</v>
@@ -5386,7 +5386,7 @@
         <v>59</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AK39" t="s" s="2">
         <v>38</v>
@@ -5394,7 +5394,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5405,7 +5405,7 @@
         <v>39</v>
       </c>
       <c r="F40" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="G40" t="s" s="2">
         <v>38</v>
@@ -5420,10 +5420,10 @@
         <v>231</v>
       </c>
       <c r="K40" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="L40" t="s" s="2">
         <v>285</v>
-      </c>
-      <c r="L40" t="s" s="2">
-        <v>286</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -5474,7 +5474,7 @@
         <v>38</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>39</v>
@@ -5500,7 +5500,7 @@
         <v>247</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C41" t="s" s="2">
         <v>38</v>
@@ -5525,13 +5525,13 @@
         <v>249</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L41" t="s" s="2">
         <v>251</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N41" t="s" s="2">
         <v>253</v>
@@ -5964,7 +5964,7 @@
         <v>38</v>
       </c>
       <c r="R45" t="s" s="2">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="S45" t="s" s="2">
         <v>38</v>
@@ -6090,7 +6090,7 @@
       </c>
       <c r="X46" s="2"/>
       <c r="Y46" t="s" s="2">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="Z46" t="s" s="2">
         <v>38</v>
@@ -6173,7 +6173,7 @@
       </c>
       <c r="P47" s="2"/>
       <c r="Q47" t="s" s="2">
-        <v>38</v>
+        <v>291</v>
       </c>
       <c r="R47" t="s" s="2">
         <v>38</v>
@@ -6230,7 +6230,7 @@
         <v>59</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AK47" t="s" s="2">
         <v>38</v>
@@ -6238,7 +6238,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -6249,7 +6249,7 @@
         <v>39</v>
       </c>
       <c r="F48" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G48" t="s" s="2">
         <v>38</v>
@@ -6264,10 +6264,10 @@
         <v>231</v>
       </c>
       <c r="K48" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="L48" t="s" s="2">
         <v>285</v>
-      </c>
-      <c r="L48" t="s" s="2">
-        <v>286</v>
       </c>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
@@ -6318,7 +6318,7 @@
         <v>38</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>39</v>
@@ -7017,7 +7017,7 @@
       </c>
       <c r="P55" s="2"/>
       <c r="Q55" t="s" s="2">
-        <v>38</v>
+        <v>291</v>
       </c>
       <c r="R55" t="s" s="2">
         <v>38</v>
@@ -7074,7 +7074,7 @@
         <v>59</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AK55" t="s" s="2">
         <v>38</v>
@@ -7082,7 +7082,7 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7093,7 +7093,7 @@
         <v>39</v>
       </c>
       <c r="F56" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G56" t="s" s="2">
         <v>38</v>
@@ -7108,10 +7108,10 @@
         <v>231</v>
       </c>
       <c r="K56" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="L56" t="s" s="2">
         <v>285</v>
-      </c>
-      <c r="L56" t="s" s="2">
-        <v>286</v>
       </c>
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
@@ -7162,7 +7162,7 @@
         <v>38</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>39</v>
@@ -7861,7 +7861,7 @@
       </c>
       <c r="P63" s="2"/>
       <c r="Q63" t="s" s="2">
-        <v>38</v>
+        <v>291</v>
       </c>
       <c r="R63" t="s" s="2">
         <v>38</v>
@@ -7918,7 +7918,7 @@
         <v>59</v>
       </c>
       <c r="AJ63" t="s" s="2">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AK63" t="s" s="2">
         <v>38</v>
@@ -7926,7 +7926,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -7937,7 +7937,7 @@
         <v>39</v>
       </c>
       <c r="F64" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G64" t="s" s="2">
         <v>38</v>
@@ -7952,10 +7952,10 @@
         <v>231</v>
       </c>
       <c r="K64" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="L64" t="s" s="2">
         <v>285</v>
-      </c>
-      <c r="L64" t="s" s="2">
-        <v>286</v>
       </c>
       <c r="M64" s="2"/>
       <c r="N64" s="2"/>
@@ -8006,7 +8006,7 @@
         <v>38</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>39</v>
@@ -8705,7 +8705,7 @@
       </c>
       <c r="P71" s="2"/>
       <c r="Q71" t="s" s="2">
-        <v>38</v>
+        <v>291</v>
       </c>
       <c r="R71" t="s" s="2">
         <v>38</v>
@@ -8762,7 +8762,7 @@
         <v>59</v>
       </c>
       <c r="AJ71" t="s" s="2">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AK71" t="s" s="2">
         <v>38</v>
@@ -8770,7 +8770,7 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -8781,7 +8781,7 @@
         <v>39</v>
       </c>
       <c r="F72" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G72" t="s" s="2">
         <v>38</v>
@@ -8796,10 +8796,10 @@
         <v>231</v>
       </c>
       <c r="K72" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="L72" t="s" s="2">
         <v>285</v>
-      </c>
-      <c r="L72" t="s" s="2">
-        <v>286</v>
       </c>
       <c r="M72" s="2"/>
       <c r="N72" s="2"/>
@@ -8850,7 +8850,7 @@
         <v>38</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>39</v>
@@ -9551,7 +9551,7 @@
       </c>
       <c r="P79" s="2"/>
       <c r="Q79" t="s" s="2">
-        <v>38</v>
+        <v>291</v>
       </c>
       <c r="R79" t="s" s="2">
         <v>38</v>
@@ -9608,7 +9608,7 @@
         <v>59</v>
       </c>
       <c r="AJ79" t="s" s="2">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AK79" t="s" s="2">
         <v>38</v>
@@ -9616,7 +9616,7 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
@@ -9627,7 +9627,7 @@
         <v>39</v>
       </c>
       <c r="F80" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G80" t="s" s="2">
         <v>38</v>
@@ -9642,10 +9642,10 @@
         <v>231</v>
       </c>
       <c r="K80" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="L80" t="s" s="2">
         <v>285</v>
-      </c>
-      <c r="L80" t="s" s="2">
-        <v>286</v>
       </c>
       <c r="M80" s="2"/>
       <c r="N80" s="2"/>
@@ -9696,7 +9696,7 @@
         <v>38</v>
       </c>
       <c r="AE80" t="s" s="2">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AF80" t="s" s="2">
         <v>39</v>

</xml_diff>